<commit_message>
cập nhật ảnh cho 20 sản phẩm
</commit_message>
<xml_diff>
--- a/CuaHangTrangSuc/productsInfo/productsData.xlsx
+++ b/CuaHangTrangSuc/productsInfo/productsData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kim Hong\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LearningInSchool\ltWeb\GitHub\CuaHangTrangSuc-Nhom4-\CuaHangTrangSuc\productsInfo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8E3B27D-7491-4E54-B4C1-8F9E48436CA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F009BF27-242A-466D-8DEE-71EBB4E56013}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CCAAE017-79D1-43DA-A5D9-A0BFA0296D81}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="504">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="479">
   <si>
     <t>id</t>
   </si>
@@ -693,39 +693,21 @@
     <t>CuaHangTrangSuc\productsInfo\products2\2.png</t>
   </si>
   <si>
-    <t>CuaHangTrangSuc\productsInfo\products2\3.png</t>
-  </si>
-  <si>
     <t>CuaHangTrangSuc\productsInfo\products2\4.png</t>
   </si>
   <si>
     <t>CuaHangTrangSuc\productsInfo\products2\5.png</t>
   </si>
   <si>
-    <t>CuaHangTrangSuc\productsInfo\products2\6.png</t>
-  </si>
-  <si>
     <t>CuaHangTrangSuc\productsInfo\products2\7.png</t>
   </si>
   <si>
     <t>CuaHangTrangSuc\productsInfo\products2\8.png</t>
   </si>
   <si>
-    <t>CuaHangTrangSuc\productsInfo\products2\9.png</t>
-  </si>
-  <si>
-    <t>CuaHangTrangSuc\productsInfo\products2\10.png</t>
-  </si>
-  <si>
     <t>CuaHangTrangSuc\productsInfo\products2\11.png</t>
   </si>
   <si>
-    <t>CuaHangTrangSuc\productsInfo\products2\12.png</t>
-  </si>
-  <si>
-    <t>CuaHangTrangSuc\productsInfo\products2\13.png</t>
-  </si>
-  <si>
     <t>CuaHangTrangSuc\productsInfo\products2\14.png</t>
   </si>
   <si>
@@ -966,33 +948,9 @@
     <t>CuaHangTrangSuc\productsInfo\products2\21.png</t>
   </si>
   <si>
-    <t>CuaHangTrangSuc\productsInfo\products2\20.png</t>
-  </si>
-  <si>
-    <t>CuaHangTrangSuc\productsInfo\products2\19.png</t>
-  </si>
-  <si>
-    <t>CuaHangTrangSuc\productsInfo\products2\18.png</t>
-  </si>
-  <si>
-    <t>CuaHangTrangSuc\productsInfo\products2\15.png</t>
-  </si>
-  <si>
-    <t>CuaHangTrangSuc\productsInfo\products2\16.png</t>
-  </si>
-  <si>
-    <t>CuaHangTrangSuc\productsInfo\products2\17.png</t>
-  </si>
-  <si>
-    <t>CuaHangTrangSuc\productsInfo\products3\1.png</t>
-  </si>
-  <si>
     <t>CuaHangTrangSuc\productsInfo\products3\2.png</t>
   </si>
   <si>
-    <t>CuaHangTrangSuc\productsInfo\products3\3.png</t>
-  </si>
-  <si>
     <t>CuaHangTrangSuc\productsInfo\products3\4.png</t>
   </si>
   <si>
@@ -1006,42 +964,6 @@
   </si>
   <si>
     <t>CuaHangTrangSuc\productsInfo\products3\8.png</t>
-  </si>
-  <si>
-    <t>CuaHangTrangSuc\productsInfo\products3\9.png</t>
-  </si>
-  <si>
-    <t>CuaHangTrangSuc\productsInfo\products3\10.png</t>
-  </si>
-  <si>
-    <t>CuaHangTrangSuc\productsInfo\products3\11.png</t>
-  </si>
-  <si>
-    <t>CuaHangTrangSuc\productsInfo\products3\12.png</t>
-  </si>
-  <si>
-    <t>CuaHangTrangSuc\productsInfo\products3\13.png</t>
-  </si>
-  <si>
-    <t>CuaHangTrangSuc\productsInfo\products3\14.png</t>
-  </si>
-  <si>
-    <t>CuaHangTrangSuc\productsInfo\products3\15.png</t>
-  </si>
-  <si>
-    <t>CuaHangTrangSuc\productsInfo\products3\16.png</t>
-  </si>
-  <si>
-    <t>CuaHangTrangSuc\productsInfo\products3\17.png</t>
-  </si>
-  <si>
-    <t>CuaHangTrangSuc\productsInfo\products3\18.png</t>
-  </si>
-  <si>
-    <t>CuaHangTrangSuc\productsInfo\products3\19.png</t>
-  </si>
-  <si>
-    <t>CuaHangTrangSuc\productsInfo\products3\20.png</t>
   </si>
   <si>
     <t>CuaHangTrangSuc\productsInfo\products3\21.png</t>
@@ -1557,6 +1479,9 @@
   </si>
   <si>
     <t>Lắc tay Bạc đính đá  Beauty &amp; The Beast ZTZTC000001</t>
+  </si>
+  <si>
+    <t>null</t>
   </si>
 </sst>
 </file>
@@ -1916,8 +1841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2D360D7-54D5-4386-A668-0103A68E7CC7}">
   <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1966,7 +1891,7 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>474</v>
+        <v>448</v>
       </c>
       <c r="D2" t="s">
         <v>117</v>
@@ -1975,7 +1900,7 @@
         <v>217</v>
       </c>
       <c r="F2" t="s">
-        <v>316</v>
+        <v>478</v>
       </c>
       <c r="G2">
         <v>655000</v>
@@ -1995,7 +1920,7 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>425</v>
+        <v>399</v>
       </c>
       <c r="D3" t="s">
         <v>122</v>
@@ -2004,7 +1929,7 @@
         <v>218</v>
       </c>
       <c r="F3" t="s">
-        <v>317</v>
+        <v>304</v>
       </c>
       <c r="G3">
         <v>6198000</v>
@@ -2024,16 +1949,16 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>426</v>
+        <v>400</v>
       </c>
       <c r="D4" t="s">
         <v>123</v>
       </c>
       <c r="E4" t="s">
-        <v>219</v>
+        <v>478</v>
       </c>
       <c r="F4" t="s">
-        <v>318</v>
+        <v>478</v>
       </c>
       <c r="G4">
         <v>1391000</v>
@@ -2053,16 +1978,16 @@
         <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>475</v>
+        <v>449</v>
       </c>
       <c r="D5" t="s">
         <v>118</v>
       </c>
       <c r="E5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F5" t="s">
-        <v>319</v>
+        <v>305</v>
       </c>
       <c r="G5">
         <v>343000</v>
@@ -2082,16 +2007,16 @@
         <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>476</v>
+        <v>450</v>
       </c>
       <c r="D6" t="s">
         <v>119</v>
       </c>
       <c r="E6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F6" t="s">
-        <v>320</v>
+        <v>306</v>
       </c>
       <c r="G6">
         <v>399000</v>
@@ -2111,16 +2036,16 @@
         <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>427</v>
+        <v>401</v>
       </c>
       <c r="D7" t="s">
         <v>124</v>
       </c>
       <c r="E7" t="s">
-        <v>222</v>
+        <v>478</v>
       </c>
       <c r="F7" t="s">
-        <v>321</v>
+        <v>307</v>
       </c>
       <c r="G7">
         <v>4888000</v>
@@ -2140,16 +2065,16 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>477</v>
+        <v>451</v>
       </c>
       <c r="D8" t="s">
         <v>120</v>
       </c>
       <c r="E8" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F8" t="s">
-        <v>322</v>
+        <v>308</v>
       </c>
       <c r="G8">
         <v>795000</v>
@@ -2169,16 +2094,16 @@
         <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>478</v>
+        <v>452</v>
       </c>
       <c r="D9" t="s">
         <v>121</v>
       </c>
       <c r="E9" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F9" t="s">
-        <v>323</v>
+        <v>309</v>
       </c>
       <c r="G9">
         <v>385000</v>
@@ -2198,19 +2123,19 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>428</v>
+        <v>402</v>
       </c>
       <c r="D10" t="s">
         <v>125</v>
       </c>
       <c r="E10" t="s">
-        <v>225</v>
+        <v>478</v>
       </c>
       <c r="F10" t="s">
-        <v>324</v>
+        <v>478</v>
       </c>
       <c r="G10" t="s">
-        <v>416</v>
+        <v>390</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -2227,16 +2152,16 @@
         <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>429</v>
+        <v>403</v>
       </c>
       <c r="D11" t="s">
         <v>126</v>
       </c>
       <c r="E11" t="s">
-        <v>226</v>
+        <v>478</v>
       </c>
       <c r="F11" t="s">
-        <v>325</v>
+        <v>478</v>
       </c>
       <c r="G11">
         <v>10848000</v>
@@ -2256,16 +2181,16 @@
         <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>430</v>
+        <v>404</v>
       </c>
       <c r="D12" t="s">
         <v>127</v>
       </c>
       <c r="E12" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="F12" t="s">
-        <v>326</v>
+        <v>478</v>
       </c>
       <c r="G12">
         <v>3941000</v>
@@ -2285,16 +2210,16 @@
         <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>431</v>
+        <v>405</v>
       </c>
       <c r="D13" t="s">
         <v>128</v>
       </c>
       <c r="E13" t="s">
-        <v>228</v>
+        <v>478</v>
       </c>
       <c r="F13" t="s">
-        <v>327</v>
+        <v>478</v>
       </c>
       <c r="G13">
         <v>4312000</v>
@@ -2314,16 +2239,16 @@
         <v>21</v>
       </c>
       <c r="C14" t="s">
-        <v>432</v>
+        <v>406</v>
       </c>
       <c r="D14" t="s">
         <v>129</v>
       </c>
       <c r="E14" t="s">
-        <v>229</v>
+        <v>478</v>
       </c>
       <c r="F14" t="s">
-        <v>328</v>
+        <v>478</v>
       </c>
       <c r="G14">
         <v>4544000</v>
@@ -2343,16 +2268,16 @@
         <v>22</v>
       </c>
       <c r="C15" t="s">
-        <v>433</v>
+        <v>407</v>
       </c>
       <c r="D15" t="s">
         <v>130</v>
       </c>
       <c r="E15" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="F15" t="s">
-        <v>329</v>
+        <v>478</v>
       </c>
       <c r="G15">
         <v>4648000</v>
@@ -2372,16 +2297,16 @@
         <v>23</v>
       </c>
       <c r="C16" t="s">
-        <v>434</v>
+        <v>408</v>
       </c>
       <c r="D16" t="s">
         <v>131</v>
       </c>
       <c r="E16" t="s">
-        <v>313</v>
+        <v>478</v>
       </c>
       <c r="F16" t="s">
-        <v>330</v>
+        <v>478</v>
       </c>
       <c r="G16">
         <v>4599000</v>
@@ -2401,16 +2326,16 @@
         <v>24</v>
       </c>
       <c r="C17" t="s">
-        <v>435</v>
+        <v>409</v>
       </c>
       <c r="D17" t="s">
         <v>132</v>
       </c>
       <c r="E17" t="s">
-        <v>314</v>
+        <v>478</v>
       </c>
       <c r="F17" t="s">
-        <v>331</v>
+        <v>478</v>
       </c>
       <c r="G17">
         <v>6001500</v>
@@ -2430,16 +2355,16 @@
         <v>25</v>
       </c>
       <c r="C18" t="s">
-        <v>436</v>
+        <v>410</v>
       </c>
       <c r="D18" t="s">
         <v>133</v>
       </c>
       <c r="E18" t="s">
-        <v>315</v>
+        <v>478</v>
       </c>
       <c r="F18" t="s">
-        <v>332</v>
+        <v>478</v>
       </c>
       <c r="G18">
         <v>7001250</v>
@@ -2459,16 +2384,16 @@
         <v>26</v>
       </c>
       <c r="C19" t="s">
-        <v>437</v>
+        <v>411</v>
       </c>
       <c r="D19" t="s">
         <v>134</v>
       </c>
       <c r="E19" t="s">
-        <v>312</v>
+        <v>478</v>
       </c>
       <c r="F19" t="s">
-        <v>333</v>
+        <v>478</v>
       </c>
       <c r="G19">
         <v>8307000</v>
@@ -2488,16 +2413,16 @@
         <v>27</v>
       </c>
       <c r="C20" t="s">
-        <v>438</v>
+        <v>412</v>
       </c>
       <c r="D20" t="s">
         <v>135</v>
       </c>
       <c r="E20" t="s">
-        <v>311</v>
+        <v>478</v>
       </c>
       <c r="F20" t="s">
-        <v>334</v>
+        <v>478</v>
       </c>
       <c r="G20">
         <v>7663000</v>
@@ -2517,16 +2442,16 @@
         <v>28</v>
       </c>
       <c r="C21" t="s">
-        <v>439</v>
+        <v>413</v>
       </c>
       <c r="D21" t="s">
         <v>145</v>
       </c>
       <c r="E21" t="s">
-        <v>310</v>
+        <v>478</v>
       </c>
       <c r="F21" t="s">
-        <v>335</v>
+        <v>478</v>
       </c>
       <c r="G21">
         <v>15330000</v>
@@ -2546,16 +2471,16 @@
         <v>29</v>
       </c>
       <c r="C22" t="s">
-        <v>440</v>
+        <v>414</v>
       </c>
       <c r="D22" t="s">
         <v>136</v>
       </c>
       <c r="E22" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="F22" t="s">
-        <v>336</v>
+        <v>310</v>
       </c>
       <c r="G22">
         <v>5687000</v>
@@ -2575,16 +2500,16 @@
         <v>30</v>
       </c>
       <c r="C23" t="s">
-        <v>441</v>
+        <v>415</v>
       </c>
       <c r="D23" t="s">
         <v>137</v>
       </c>
       <c r="E23" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="F23" t="s">
-        <v>337</v>
+        <v>311</v>
       </c>
       <c r="G23">
         <v>13600000</v>
@@ -2604,16 +2529,16 @@
         <v>31</v>
       </c>
       <c r="C24" t="s">
-        <v>442</v>
+        <v>416</v>
       </c>
       <c r="D24" t="s">
         <v>138</v>
       </c>
       <c r="E24" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="F24" t="s">
-        <v>338</v>
+        <v>312</v>
       </c>
       <c r="G24">
         <v>15943000</v>
@@ -2633,16 +2558,16 @@
         <v>32</v>
       </c>
       <c r="C25" t="s">
-        <v>443</v>
+        <v>417</v>
       </c>
       <c r="D25" t="s">
         <v>139</v>
       </c>
       <c r="E25" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="F25" t="s">
-        <v>339</v>
+        <v>313</v>
       </c>
       <c r="G25">
         <v>15540000</v>
@@ -2662,16 +2587,16 @@
         <v>33</v>
       </c>
       <c r="C26" t="s">
-        <v>444</v>
+        <v>418</v>
       </c>
       <c r="D26" t="s">
         <v>140</v>
       </c>
       <c r="E26" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="F26" t="s">
-        <v>340</v>
+        <v>314</v>
       </c>
       <c r="G26">
         <v>16586000</v>
@@ -2691,16 +2616,16 @@
         <v>34</v>
       </c>
       <c r="C27" t="s">
-        <v>445</v>
+        <v>419</v>
       </c>
       <c r="D27" t="s">
         <v>141</v>
       </c>
       <c r="E27" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="F27" t="s">
-        <v>341</v>
+        <v>315</v>
       </c>
       <c r="G27">
         <v>9558000</v>
@@ -2720,16 +2645,16 @@
         <v>35</v>
       </c>
       <c r="C28" t="s">
-        <v>446</v>
+        <v>420</v>
       </c>
       <c r="D28" t="s">
         <v>142</v>
       </c>
       <c r="E28" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="F28" t="s">
-        <v>342</v>
+        <v>316</v>
       </c>
       <c r="G28">
         <v>11792000</v>
@@ -2749,16 +2674,16 @@
         <v>36</v>
       </c>
       <c r="C29" t="s">
-        <v>447</v>
+        <v>421</v>
       </c>
       <c r="D29" t="s">
         <v>143</v>
       </c>
       <c r="E29" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="F29" t="s">
-        <v>343</v>
+        <v>317</v>
       </c>
       <c r="G29">
         <v>14030000</v>
@@ -2778,16 +2703,16 @@
         <v>37</v>
       </c>
       <c r="C30" t="s">
-        <v>448</v>
+        <v>422</v>
       </c>
       <c r="D30" t="s">
         <v>144</v>
       </c>
       <c r="E30" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="F30" t="s">
-        <v>344</v>
+        <v>318</v>
       </c>
       <c r="G30">
         <v>15348000</v>
@@ -2807,16 +2732,16 @@
         <v>38</v>
       </c>
       <c r="C31" t="s">
-        <v>449</v>
+        <v>423</v>
       </c>
       <c r="D31" t="s">
         <v>153</v>
       </c>
       <c r="E31" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="F31" t="s">
-        <v>345</v>
+        <v>319</v>
       </c>
       <c r="G31">
         <v>6185000</v>
@@ -2836,16 +2761,16 @@
         <v>39</v>
       </c>
       <c r="C32" t="s">
-        <v>479</v>
+        <v>453</v>
       </c>
       <c r="D32" t="s">
         <v>154</v>
       </c>
       <c r="E32" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="F32" t="s">
-        <v>346</v>
+        <v>320</v>
       </c>
       <c r="G32">
         <v>257000</v>
@@ -2865,16 +2790,16 @@
         <v>40</v>
       </c>
       <c r="C33" t="s">
-        <v>480</v>
+        <v>454</v>
       </c>
       <c r="D33" t="s">
         <v>155</v>
       </c>
       <c r="E33" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="F33" t="s">
-        <v>347</v>
+        <v>321</v>
       </c>
       <c r="G33">
         <v>609000</v>
@@ -2894,16 +2819,16 @@
         <v>41</v>
       </c>
       <c r="C34" t="s">
-        <v>481</v>
+        <v>455</v>
       </c>
       <c r="D34" t="s">
         <v>156</v>
       </c>
       <c r="E34" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="F34" t="s">
-        <v>348</v>
+        <v>322</v>
       </c>
       <c r="G34">
         <v>537000</v>
@@ -2923,16 +2848,16 @@
         <v>42</v>
       </c>
       <c r="C35" t="s">
-        <v>482</v>
+        <v>456</v>
       </c>
       <c r="D35" t="s">
         <v>157</v>
       </c>
       <c r="E35" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="F35" t="s">
-        <v>349</v>
+        <v>323</v>
       </c>
       <c r="G35">
         <v>525000</v>
@@ -2952,16 +2877,16 @@
         <v>43</v>
       </c>
       <c r="C36" t="s">
-        <v>483</v>
+        <v>457</v>
       </c>
       <c r="D36" t="s">
         <v>158</v>
       </c>
       <c r="E36" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="F36" t="s">
-        <v>350</v>
+        <v>324</v>
       </c>
       <c r="G36">
         <v>635000</v>
@@ -2981,16 +2906,16 @@
         <v>44</v>
       </c>
       <c r="C37" t="s">
-        <v>450</v>
+        <v>424</v>
       </c>
       <c r="D37" t="s">
         <v>159</v>
       </c>
       <c r="E37" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="F37" t="s">
-        <v>351</v>
+        <v>325</v>
       </c>
       <c r="G37">
         <v>2621000</v>
@@ -3010,16 +2935,16 @@
         <v>45</v>
       </c>
       <c r="C38" t="s">
-        <v>451</v>
+        <v>425</v>
       </c>
       <c r="D38" t="s">
         <v>160</v>
       </c>
       <c r="E38" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="F38" t="s">
-        <v>352</v>
+        <v>326</v>
       </c>
       <c r="G38">
         <v>5556000</v>
@@ -3039,16 +2964,16 @@
         <v>46</v>
       </c>
       <c r="C39" t="s">
-        <v>452</v>
+        <v>426</v>
       </c>
       <c r="D39" t="s">
         <v>161</v>
       </c>
       <c r="E39" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="F39" t="s">
-        <v>353</v>
+        <v>327</v>
       </c>
       <c r="G39">
         <v>6701000</v>
@@ -3068,16 +2993,16 @@
         <v>47</v>
       </c>
       <c r="C40" t="s">
-        <v>453</v>
+        <v>427</v>
       </c>
       <c r="D40" t="s">
         <v>162</v>
       </c>
       <c r="E40" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="F40" t="s">
-        <v>354</v>
+        <v>328</v>
       </c>
       <c r="G40">
         <v>9058000</v>
@@ -3097,16 +3022,16 @@
         <v>48</v>
       </c>
       <c r="C41" t="s">
-        <v>454</v>
+        <v>428</v>
       </c>
       <c r="D41" t="s">
         <v>146</v>
       </c>
       <c r="E41" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="F41" t="s">
-        <v>355</v>
+        <v>329</v>
       </c>
       <c r="G41">
         <v>3964000</v>
@@ -3126,7 +3051,7 @@
         <v>49</v>
       </c>
       <c r="C42" t="s">
-        <v>484</v>
+        <v>458</v>
       </c>
       <c r="D42" t="s">
         <v>147</v>
@@ -3135,7 +3060,7 @@
         <v>147</v>
       </c>
       <c r="F42" t="s">
-        <v>356</v>
+        <v>330</v>
       </c>
       <c r="G42">
         <v>485000</v>
@@ -3155,16 +3080,16 @@
         <v>50</v>
       </c>
       <c r="C43" t="s">
-        <v>485</v>
+        <v>459</v>
       </c>
       <c r="D43" t="s">
         <v>148</v>
       </c>
       <c r="E43" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="F43" t="s">
-        <v>357</v>
+        <v>331</v>
       </c>
       <c r="G43">
         <v>427000</v>
@@ -3184,16 +3109,16 @@
         <v>51</v>
       </c>
       <c r="C44" t="s">
-        <v>486</v>
+        <v>460</v>
       </c>
       <c r="D44" t="s">
         <v>149</v>
       </c>
       <c r="E44" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="F44" t="s">
-        <v>358</v>
+        <v>332</v>
       </c>
       <c r="G44">
         <v>551000</v>
@@ -3213,16 +3138,16 @@
         <v>52</v>
       </c>
       <c r="C45" t="s">
-        <v>487</v>
+        <v>461</v>
       </c>
       <c r="D45" t="s">
         <v>150</v>
       </c>
       <c r="E45" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="F45" t="s">
-        <v>359</v>
+        <v>333</v>
       </c>
       <c r="G45">
         <v>639000</v>
@@ -3242,16 +3167,16 @@
         <v>53</v>
       </c>
       <c r="C46" t="s">
-        <v>488</v>
+        <v>462</v>
       </c>
       <c r="D46" t="s">
         <v>151</v>
       </c>
       <c r="E46" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="F46" t="s">
-        <v>360</v>
+        <v>334</v>
       </c>
       <c r="G46">
         <v>661000</v>
@@ -3271,16 +3196,16 @@
         <v>54</v>
       </c>
       <c r="C47" t="s">
-        <v>489</v>
+        <v>463</v>
       </c>
       <c r="D47" t="s">
         <v>152</v>
       </c>
       <c r="E47" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="F47" t="s">
-        <v>361</v>
+        <v>335</v>
       </c>
       <c r="G47">
         <v>673000</v>
@@ -3300,16 +3225,16 @@
         <v>55</v>
       </c>
       <c r="C48" t="s">
-        <v>490</v>
+        <v>464</v>
       </c>
       <c r="D48" t="s">
         <v>163</v>
       </c>
       <c r="E48" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="F48" t="s">
-        <v>362</v>
+        <v>336</v>
       </c>
       <c r="G48">
         <v>445000</v>
@@ -3329,16 +3254,16 @@
         <v>56</v>
       </c>
       <c r="C49" t="s">
-        <v>491</v>
+        <v>465</v>
       </c>
       <c r="D49" t="s">
         <v>164</v>
       </c>
       <c r="E49" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="F49" t="s">
-        <v>363</v>
+        <v>337</v>
       </c>
       <c r="G49">
         <v>498000</v>
@@ -3358,16 +3283,16 @@
         <v>57</v>
       </c>
       <c r="C50" t="s">
-        <v>492</v>
+        <v>466</v>
       </c>
       <c r="D50" t="s">
         <v>165</v>
       </c>
       <c r="E50" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="F50" t="s">
-        <v>364</v>
+        <v>338</v>
       </c>
       <c r="G50">
         <v>546000</v>
@@ -3387,16 +3312,16 @@
         <v>58</v>
       </c>
       <c r="C51" t="s">
-        <v>493</v>
+        <v>467</v>
       </c>
       <c r="D51" t="s">
         <v>166</v>
       </c>
       <c r="E51" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="F51" t="s">
-        <v>365</v>
+        <v>339</v>
       </c>
       <c r="G51">
         <v>945000</v>
@@ -3416,16 +3341,16 @@
         <v>59</v>
       </c>
       <c r="C52" t="s">
-        <v>501</v>
+        <v>475</v>
       </c>
       <c r="D52" t="s">
         <v>213</v>
       </c>
       <c r="E52" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="F52" t="s">
-        <v>366</v>
+        <v>340</v>
       </c>
       <c r="G52">
         <v>1295000</v>
@@ -3445,16 +3370,16 @@
         <v>60</v>
       </c>
       <c r="C53" t="s">
-        <v>494</v>
+        <v>468</v>
       </c>
       <c r="D53" t="s">
         <v>167</v>
       </c>
       <c r="E53" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="F53" t="s">
-        <v>367</v>
+        <v>341</v>
       </c>
       <c r="G53">
         <v>857000</v>
@@ -3474,16 +3399,16 @@
         <v>61</v>
       </c>
       <c r="C54" t="s">
-        <v>495</v>
+        <v>469</v>
       </c>
       <c r="D54" t="s">
         <v>168</v>
       </c>
       <c r="E54" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="F54" t="s">
-        <v>368</v>
+        <v>342</v>
       </c>
       <c r="G54">
         <v>1045000</v>
@@ -3503,16 +3428,16 @@
         <v>62</v>
       </c>
       <c r="C55" t="s">
-        <v>496</v>
+        <v>470</v>
       </c>
       <c r="D55" t="s">
         <v>169</v>
       </c>
       <c r="E55" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="F55" t="s">
-        <v>369</v>
+        <v>343</v>
       </c>
       <c r="G55">
         <v>895000</v>
@@ -3532,16 +3457,16 @@
         <v>63</v>
       </c>
       <c r="C56" t="s">
-        <v>502</v>
+        <v>476</v>
       </c>
       <c r="D56" t="s">
         <v>170</v>
       </c>
       <c r="E56" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="F56" t="s">
-        <v>370</v>
+        <v>344</v>
       </c>
       <c r="G56">
         <v>1585000</v>
@@ -3561,16 +3486,16 @@
         <v>64</v>
       </c>
       <c r="C57" t="s">
-        <v>497</v>
+        <v>471</v>
       </c>
       <c r="D57" t="s">
         <v>171</v>
       </c>
       <c r="E57" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="F57" t="s">
-        <v>371</v>
+        <v>345</v>
       </c>
       <c r="G57">
         <v>1335000</v>
@@ -3590,16 +3515,16 @@
         <v>65</v>
       </c>
       <c r="C58" t="s">
-        <v>503</v>
+        <v>477</v>
       </c>
       <c r="D58" t="s">
         <v>172</v>
       </c>
       <c r="E58" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="F58" t="s">
-        <v>372</v>
+        <v>346</v>
       </c>
       <c r="G58">
         <v>1355000</v>
@@ -3619,16 +3544,16 @@
         <v>66</v>
       </c>
       <c r="C59" t="s">
-        <v>498</v>
+        <v>472</v>
       </c>
       <c r="D59" t="s">
         <v>173</v>
       </c>
       <c r="E59" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="F59" t="s">
-        <v>373</v>
+        <v>347</v>
       </c>
       <c r="G59">
         <v>745000</v>
@@ -3648,16 +3573,16 @@
         <v>67</v>
       </c>
       <c r="C60" t="s">
-        <v>499</v>
+        <v>473</v>
       </c>
       <c r="D60" t="s">
         <v>174</v>
       </c>
       <c r="E60" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="F60" t="s">
-        <v>374</v>
+        <v>348</v>
       </c>
       <c r="G60">
         <v>471000</v>
@@ -3677,16 +3602,16 @@
         <v>68</v>
       </c>
       <c r="C61" t="s">
-        <v>500</v>
+        <v>474</v>
       </c>
       <c r="D61" t="s">
         <v>175</v>
       </c>
       <c r="E61" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="F61" t="s">
-        <v>375</v>
+        <v>349</v>
       </c>
       <c r="G61">
         <v>1085000</v>
@@ -3703,7 +3628,7 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>417</v>
+        <v>391</v>
       </c>
       <c r="C62" t="s">
         <v>99</v>
@@ -3712,10 +3637,10 @@
         <v>176</v>
       </c>
       <c r="E62" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="F62" t="s">
-        <v>376</v>
+        <v>350</v>
       </c>
       <c r="G62">
         <v>2468000</v>
@@ -3741,10 +3666,10 @@
         <v>177</v>
       </c>
       <c r="E63" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="F63" t="s">
-        <v>377</v>
+        <v>351</v>
       </c>
       <c r="H63">
         <v>4</v>
@@ -3758,7 +3683,7 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>418</v>
+        <v>392</v>
       </c>
       <c r="C64" t="s">
         <v>101</v>
@@ -3767,10 +3692,10 @@
         <v>178</v>
       </c>
       <c r="E64" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="F64" t="s">
-        <v>378</v>
+        <v>352</v>
       </c>
       <c r="G64">
         <v>8785000</v>
@@ -3787,7 +3712,7 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>419</v>
+        <v>393</v>
       </c>
       <c r="C65" t="s">
         <v>102</v>
@@ -3796,10 +3721,10 @@
         <v>179</v>
       </c>
       <c r="E65" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="F65" t="s">
-        <v>379</v>
+        <v>353</v>
       </c>
       <c r="G65">
         <v>8930000</v>
@@ -3816,7 +3741,7 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>420</v>
+        <v>394</v>
       </c>
       <c r="C66" t="s">
         <v>103</v>
@@ -3825,10 +3750,10 @@
         <v>180</v>
       </c>
       <c r="E66" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="F66" t="s">
-        <v>380</v>
+        <v>354</v>
       </c>
       <c r="G66">
         <v>7970000</v>
@@ -3854,10 +3779,10 @@
         <v>181</v>
       </c>
       <c r="E67" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F67" t="s">
-        <v>381</v>
+        <v>355</v>
       </c>
       <c r="G67">
         <v>2670000</v>
@@ -3874,7 +3799,7 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>421</v>
+        <v>395</v>
       </c>
       <c r="C68" t="s">
         <v>105</v>
@@ -3883,10 +3808,10 @@
         <v>182</v>
       </c>
       <c r="E68" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="F68" t="s">
-        <v>382</v>
+        <v>356</v>
       </c>
       <c r="G68">
         <v>5420000</v>
@@ -3903,7 +3828,7 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>422</v>
+        <v>396</v>
       </c>
       <c r="C69" t="s">
         <v>106</v>
@@ -3912,10 +3837,10 @@
         <v>183</v>
       </c>
       <c r="E69" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="F69" t="s">
-        <v>383</v>
+        <v>357</v>
       </c>
       <c r="G69">
         <v>4550000</v>
@@ -3932,7 +3857,7 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>423</v>
+        <v>397</v>
       </c>
       <c r="C70" t="s">
         <v>107</v>
@@ -3941,10 +3866,10 @@
         <v>184</v>
       </c>
       <c r="E70" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="F70" t="s">
-        <v>384</v>
+        <v>358</v>
       </c>
       <c r="G70">
         <v>4840000</v>
@@ -3961,7 +3886,7 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>424</v>
+        <v>398</v>
       </c>
       <c r="C71" t="s">
         <v>108</v>
@@ -3970,10 +3895,10 @@
         <v>185</v>
       </c>
       <c r="E71" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="F71" t="s">
-        <v>385</v>
+        <v>359</v>
       </c>
       <c r="G71">
         <v>4530000</v>
@@ -3999,10 +3924,10 @@
         <v>186</v>
       </c>
       <c r="E72" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="F72" t="s">
-        <v>386</v>
+        <v>360</v>
       </c>
       <c r="G72">
         <v>2400000</v>
@@ -4028,10 +3953,10 @@
         <v>187</v>
       </c>
       <c r="E73" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="F73" t="s">
-        <v>387</v>
+        <v>361</v>
       </c>
       <c r="G73">
         <v>2360000</v>
@@ -4057,10 +3982,10 @@
         <v>188</v>
       </c>
       <c r="E74" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="F74" t="s">
-        <v>388</v>
+        <v>362</v>
       </c>
       <c r="G74">
         <v>2468000</v>
@@ -4086,10 +4011,10 @@
         <v>189</v>
       </c>
       <c r="E75" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="F75" t="s">
-        <v>389</v>
+        <v>363</v>
       </c>
       <c r="G75">
         <v>2468000</v>
@@ -4115,10 +4040,10 @@
         <v>190</v>
       </c>
       <c r="E76" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="F76" t="s">
-        <v>390</v>
+        <v>364</v>
       </c>
       <c r="G76">
         <v>2468000</v>
@@ -4144,10 +4069,10 @@
         <v>191</v>
       </c>
       <c r="E77" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="F77" t="s">
-        <v>391</v>
+        <v>365</v>
       </c>
       <c r="G77">
         <v>2562000</v>
@@ -4173,10 +4098,10 @@
         <v>192</v>
       </c>
       <c r="E78" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="F78" t="s">
-        <v>392</v>
+        <v>366</v>
       </c>
       <c r="G78">
         <v>2562000</v>
@@ -4202,10 +4127,10 @@
         <v>193</v>
       </c>
       <c r="E79" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="F79" t="s">
-        <v>393</v>
+        <v>367</v>
       </c>
       <c r="G79">
         <v>2670000</v>
@@ -4231,10 +4156,10 @@
         <v>194</v>
       </c>
       <c r="E80" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="F80" t="s">
-        <v>394</v>
+        <v>368</v>
       </c>
       <c r="G80">
         <v>2773000</v>
@@ -4260,10 +4185,10 @@
         <v>195</v>
       </c>
       <c r="E81" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="F81" t="s">
-        <v>395</v>
+        <v>369</v>
       </c>
       <c r="G81">
         <v>2773000</v>
@@ -4289,10 +4214,10 @@
         <v>196</v>
       </c>
       <c r="E82" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="F82" t="s">
-        <v>396</v>
+        <v>370</v>
       </c>
       <c r="G82">
         <v>2810000</v>
@@ -4312,16 +4237,16 @@
         <v>80</v>
       </c>
       <c r="C83" t="s">
-        <v>455</v>
+        <v>429</v>
       </c>
       <c r="D83" t="s">
         <v>197</v>
       </c>
       <c r="E83" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="F83" t="s">
-        <v>397</v>
+        <v>371</v>
       </c>
       <c r="G83">
         <v>1080000</v>
@@ -4341,16 +4266,16 @@
         <v>81</v>
       </c>
       <c r="C84" t="s">
-        <v>456</v>
+        <v>430</v>
       </c>
       <c r="D84" t="s">
         <v>198</v>
       </c>
       <c r="E84" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="F84" t="s">
-        <v>398</v>
+        <v>372</v>
       </c>
       <c r="G84">
         <v>1322000</v>
@@ -4370,16 +4295,16 @@
         <v>82</v>
       </c>
       <c r="C85" t="s">
-        <v>457</v>
+        <v>431</v>
       </c>
       <c r="D85" t="s">
         <v>199</v>
       </c>
       <c r="E85" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="F85" t="s">
-        <v>399</v>
+        <v>373</v>
       </c>
       <c r="G85">
         <v>1717000</v>
@@ -4399,16 +4324,16 @@
         <v>83</v>
       </c>
       <c r="C86" t="s">
-        <v>458</v>
+        <v>432</v>
       </c>
       <c r="D86" t="s">
         <v>200</v>
       </c>
       <c r="E86" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="F86" t="s">
-        <v>400</v>
+        <v>374</v>
       </c>
       <c r="G86">
         <v>2341000</v>
@@ -4428,16 +4353,16 @@
         <v>84</v>
       </c>
       <c r="C87" t="s">
-        <v>459</v>
+        <v>433</v>
       </c>
       <c r="D87" t="s">
         <v>201</v>
       </c>
       <c r="E87" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="F87" t="s">
-        <v>401</v>
+        <v>375</v>
       </c>
       <c r="G87">
         <v>2175000</v>
@@ -4457,16 +4382,16 @@
         <v>85</v>
       </c>
       <c r="C88" t="s">
-        <v>460</v>
+        <v>434</v>
       </c>
       <c r="D88" t="s">
         <v>202</v>
       </c>
       <c r="E88" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="F88" t="s">
-        <v>402</v>
+        <v>376</v>
       </c>
       <c r="G88">
         <v>1862000</v>
@@ -4486,16 +4411,16 @@
         <v>86</v>
       </c>
       <c r="C89" t="s">
-        <v>461</v>
+        <v>435</v>
       </c>
       <c r="D89" t="s">
         <v>203</v>
       </c>
       <c r="E89" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="F89" t="s">
-        <v>403</v>
+        <v>377</v>
       </c>
       <c r="G89">
         <v>6713000</v>
@@ -4515,16 +4440,16 @@
         <v>87</v>
       </c>
       <c r="C90" t="s">
-        <v>462</v>
+        <v>436</v>
       </c>
       <c r="D90" t="s">
         <v>204</v>
       </c>
       <c r="E90" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="F90" t="s">
-        <v>404</v>
+        <v>378</v>
       </c>
       <c r="G90">
         <v>6627000</v>
@@ -4544,16 +4469,16 @@
         <v>88</v>
       </c>
       <c r="C91" t="s">
-        <v>463</v>
+        <v>437</v>
       </c>
       <c r="D91" t="s">
         <v>205</v>
       </c>
       <c r="E91" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="F91" t="s">
-        <v>405</v>
+        <v>379</v>
       </c>
       <c r="G91">
         <v>20615000</v>
@@ -4573,16 +4498,16 @@
         <v>89</v>
       </c>
       <c r="C92" t="s">
-        <v>464</v>
+        <v>438</v>
       </c>
       <c r="D92" t="s">
         <v>206</v>
       </c>
       <c r="E92" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="F92" t="s">
-        <v>406</v>
+        <v>380</v>
       </c>
       <c r="G92">
         <v>9275000</v>
@@ -4602,16 +4527,16 @@
         <v>90</v>
       </c>
       <c r="C93" t="s">
-        <v>465</v>
+        <v>439</v>
       </c>
       <c r="D93" t="s">
         <v>207</v>
       </c>
       <c r="E93" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="F93" t="s">
-        <v>407</v>
+        <v>381</v>
       </c>
       <c r="G93">
         <v>10326000</v>
@@ -4631,16 +4556,16 @@
         <v>91</v>
       </c>
       <c r="C94" t="s">
-        <v>466</v>
+        <v>440</v>
       </c>
       <c r="D94" t="s">
         <v>208</v>
       </c>
       <c r="E94" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="F94" t="s">
-        <v>408</v>
+        <v>382</v>
       </c>
       <c r="G94">
         <v>10691000</v>
@@ -4660,16 +4585,16 @@
         <v>92</v>
       </c>
       <c r="C95" t="s">
-        <v>467</v>
+        <v>441</v>
       </c>
       <c r="D95" t="s">
         <v>209</v>
       </c>
       <c r="E95" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="F95" t="s">
-        <v>409</v>
+        <v>383</v>
       </c>
       <c r="G95">
         <v>68528000</v>
@@ -4689,16 +4614,16 @@
         <v>93</v>
       </c>
       <c r="C96" t="s">
-        <v>468</v>
+        <v>442</v>
       </c>
       <c r="D96" t="s">
         <v>210</v>
       </c>
       <c r="E96" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="F96" t="s">
-        <v>410</v>
+        <v>384</v>
       </c>
       <c r="G96">
         <v>10342000</v>
@@ -4718,16 +4643,16 @@
         <v>94</v>
       </c>
       <c r="C97" t="s">
-        <v>469</v>
+        <v>443</v>
       </c>
       <c r="D97" t="s">
         <v>211</v>
       </c>
       <c r="E97" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="F97" t="s">
-        <v>411</v>
+        <v>385</v>
       </c>
       <c r="G97">
         <v>2441000</v>
@@ -4747,16 +4672,16 @@
         <v>95</v>
       </c>
       <c r="C98" t="s">
-        <v>470</v>
+        <v>444</v>
       </c>
       <c r="D98" t="s">
         <v>214</v>
       </c>
       <c r="E98" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="F98" t="s">
-        <v>412</v>
+        <v>386</v>
       </c>
       <c r="G98">
         <v>1826000</v>
@@ -4776,16 +4701,16 @@
         <v>96</v>
       </c>
       <c r="C99" t="s">
-        <v>471</v>
+        <v>445</v>
       </c>
       <c r="D99" t="s">
         <v>215</v>
       </c>
       <c r="E99" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="F99" t="s">
-        <v>413</v>
+        <v>387</v>
       </c>
       <c r="G99">
         <v>2450000</v>
@@ -4805,16 +4730,16 @@
         <v>97</v>
       </c>
       <c r="C100" t="s">
-        <v>472</v>
+        <v>446</v>
       </c>
       <c r="D100" t="s">
         <v>216</v>
       </c>
       <c r="E100" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="F100" t="s">
-        <v>414</v>
+        <v>388</v>
       </c>
       <c r="G100">
         <v>10346000</v>
@@ -4834,16 +4759,16 @@
         <v>98</v>
       </c>
       <c r="C101" t="s">
-        <v>473</v>
+        <v>447</v>
       </c>
       <c r="D101" t="s">
         <v>212</v>
       </c>
       <c r="E101" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="F101" t="s">
-        <v>415</v>
+        <v>389</v>
       </c>
       <c r="G101">
         <v>5723000</v>

</xml_diff>

<commit_message>
update ảnh cho 20 sản phẩm
</commit_message>
<xml_diff>
--- a/CuaHangTrangSuc/productsInfo/productsData.xlsx
+++ b/CuaHangTrangSuc/productsInfo/productsData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LearningInSchool\ltWeb\GitHub\CuaHangTrangSuc-Nhom4-\CuaHangTrangSuc\productsInfo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F009BF27-242A-466D-8DEE-71EBB4E56013}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{410F1E47-9C18-4200-ACD6-085ACFD10BE2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CCAAE017-79D1-43DA-A5D9-A0BFA0296D81}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="466">
   <si>
     <t>id</t>
   </si>
@@ -894,12 +894,6 @@
     <t>CuaHangTrangSuc\productsInfo\products2\39.png</t>
   </si>
   <si>
-    <t>CuaHangTrangSuc\productsInfo\products2\38.png</t>
-  </si>
-  <si>
-    <t>CuaHangTrangSuc\productsInfo\products2\37.png</t>
-  </si>
-  <si>
     <t>CuaHangTrangSuc\productsInfo\products2\36.png</t>
   </si>
   <si>
@@ -912,9 +906,6 @@
     <t>CuaHangTrangSuc\productsInfo\products2\33.png</t>
   </si>
   <si>
-    <t>CuaHangTrangSuc\productsInfo\products2\32.png</t>
-  </si>
-  <si>
     <t>CuaHangTrangSuc\productsInfo\products2\31.png</t>
   </si>
   <si>
@@ -930,15 +921,9 @@
     <t>CuaHangTrangSuc\productsInfo\products2\27.png</t>
   </si>
   <si>
-    <t>CuaHangTrangSuc\productsInfo\products2\26.png</t>
-  </si>
-  <si>
     <t>CuaHangTrangSuc\productsInfo\products2\25.png</t>
   </si>
   <si>
-    <t>CuaHangTrangSuc\productsInfo\products2\24.png</t>
-  </si>
-  <si>
     <t>CuaHangTrangSuc\productsInfo\products2\23.png</t>
   </si>
   <si>
@@ -966,24 +951,12 @@
     <t>CuaHangTrangSuc\productsInfo\products3\8.png</t>
   </si>
   <si>
-    <t>CuaHangTrangSuc\productsInfo\products3\21.png</t>
-  </si>
-  <si>
     <t>CuaHangTrangSuc\productsInfo\products3\22.png</t>
   </si>
   <si>
-    <t>CuaHangTrangSuc\productsInfo\products3\23.png</t>
-  </si>
-  <si>
-    <t>CuaHangTrangSuc\productsInfo\products3\24.png</t>
-  </si>
-  <si>
     <t>CuaHangTrangSuc\productsInfo\products3\25.png</t>
   </si>
   <si>
-    <t>CuaHangTrangSuc\productsInfo\products3\26.png</t>
-  </si>
-  <si>
     <t>CuaHangTrangSuc\productsInfo\products3\27.png</t>
   </si>
   <si>
@@ -999,12 +972,6 @@
     <t>CuaHangTrangSuc\productsInfo\products3\31.png</t>
   </si>
   <si>
-    <t>CuaHangTrangSuc\productsInfo\products3\32.png</t>
-  </si>
-  <si>
-    <t>CuaHangTrangSuc\productsInfo\products3\33.png</t>
-  </si>
-  <si>
     <t>CuaHangTrangSuc\productsInfo\products3\34.png</t>
   </si>
   <si>
@@ -1012,12 +979,6 @@
   </si>
   <si>
     <t>CuaHangTrangSuc\productsInfo\products3\36.png</t>
-  </si>
-  <si>
-    <t>CuaHangTrangSuc\productsInfo\products3\37.png</t>
-  </si>
-  <si>
-    <t>CuaHangTrangSuc\productsInfo\products3\38.png</t>
   </si>
   <si>
     <t>CuaHangTrangSuc\productsInfo\products3\39.png</t>
@@ -1841,8 +1802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2D360D7-54D5-4386-A668-0103A68E7CC7}">
   <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="C31" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1891,7 +1852,7 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>448</v>
+        <v>435</v>
       </c>
       <c r="D2" t="s">
         <v>117</v>
@@ -1900,7 +1861,7 @@
         <v>217</v>
       </c>
       <c r="F2" t="s">
-        <v>478</v>
+        <v>465</v>
       </c>
       <c r="G2">
         <v>655000</v>
@@ -1920,7 +1881,7 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>399</v>
+        <v>386</v>
       </c>
       <c r="D3" t="s">
         <v>122</v>
@@ -1929,7 +1890,7 @@
         <v>218</v>
       </c>
       <c r="F3" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="G3">
         <v>6198000</v>
@@ -1949,16 +1910,16 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>400</v>
+        <v>387</v>
       </c>
       <c r="D4" t="s">
         <v>123</v>
       </c>
       <c r="E4" t="s">
-        <v>478</v>
+        <v>465</v>
       </c>
       <c r="F4" t="s">
-        <v>478</v>
+        <v>465</v>
       </c>
       <c r="G4">
         <v>1391000</v>
@@ -1978,7 +1939,7 @@
         <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>449</v>
+        <v>436</v>
       </c>
       <c r="D5" t="s">
         <v>118</v>
@@ -1987,7 +1948,7 @@
         <v>219</v>
       </c>
       <c r="F5" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="G5">
         <v>343000</v>
@@ -2007,7 +1968,7 @@
         <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>450</v>
+        <v>437</v>
       </c>
       <c r="D6" t="s">
         <v>119</v>
@@ -2016,7 +1977,7 @@
         <v>220</v>
       </c>
       <c r="F6" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="G6">
         <v>399000</v>
@@ -2036,16 +1997,16 @@
         <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>401</v>
+        <v>388</v>
       </c>
       <c r="D7" t="s">
         <v>124</v>
       </c>
       <c r="E7" t="s">
-        <v>478</v>
+        <v>465</v>
       </c>
       <c r="F7" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="G7">
         <v>4888000</v>
@@ -2065,7 +2026,7 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>451</v>
+        <v>438</v>
       </c>
       <c r="D8" t="s">
         <v>120</v>
@@ -2074,7 +2035,7 @@
         <v>221</v>
       </c>
       <c r="F8" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="G8">
         <v>795000</v>
@@ -2094,7 +2055,7 @@
         <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>452</v>
+        <v>439</v>
       </c>
       <c r="D9" t="s">
         <v>121</v>
@@ -2103,7 +2064,7 @@
         <v>222</v>
       </c>
       <c r="F9" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="G9">
         <v>385000</v>
@@ -2123,19 +2084,19 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>402</v>
+        <v>389</v>
       </c>
       <c r="D10" t="s">
         <v>125</v>
       </c>
       <c r="E10" t="s">
-        <v>478</v>
+        <v>465</v>
       </c>
       <c r="F10" t="s">
-        <v>478</v>
+        <v>465</v>
       </c>
       <c r="G10" t="s">
-        <v>390</v>
+        <v>377</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -2152,16 +2113,16 @@
         <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>403</v>
+        <v>390</v>
       </c>
       <c r="D11" t="s">
         <v>126</v>
       </c>
       <c r="E11" t="s">
-        <v>478</v>
+        <v>465</v>
       </c>
       <c r="F11" t="s">
-        <v>478</v>
+        <v>465</v>
       </c>
       <c r="G11">
         <v>10848000</v>
@@ -2181,7 +2142,7 @@
         <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>404</v>
+        <v>391</v>
       </c>
       <c r="D12" t="s">
         <v>127</v>
@@ -2190,7 +2151,7 @@
         <v>223</v>
       </c>
       <c r="F12" t="s">
-        <v>478</v>
+        <v>465</v>
       </c>
       <c r="G12">
         <v>3941000</v>
@@ -2210,16 +2171,16 @@
         <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>405</v>
+        <v>392</v>
       </c>
       <c r="D13" t="s">
         <v>128</v>
       </c>
       <c r="E13" t="s">
-        <v>478</v>
+        <v>465</v>
       </c>
       <c r="F13" t="s">
-        <v>478</v>
+        <v>465</v>
       </c>
       <c r="G13">
         <v>4312000</v>
@@ -2239,16 +2200,16 @@
         <v>21</v>
       </c>
       <c r="C14" t="s">
-        <v>406</v>
+        <v>393</v>
       </c>
       <c r="D14" t="s">
         <v>129</v>
       </c>
       <c r="E14" t="s">
-        <v>478</v>
+        <v>465</v>
       </c>
       <c r="F14" t="s">
-        <v>478</v>
+        <v>465</v>
       </c>
       <c r="G14">
         <v>4544000</v>
@@ -2268,7 +2229,7 @@
         <v>22</v>
       </c>
       <c r="C15" t="s">
-        <v>407</v>
+        <v>394</v>
       </c>
       <c r="D15" t="s">
         <v>130</v>
@@ -2277,7 +2238,7 @@
         <v>224</v>
       </c>
       <c r="F15" t="s">
-        <v>478</v>
+        <v>465</v>
       </c>
       <c r="G15">
         <v>4648000</v>
@@ -2297,16 +2258,16 @@
         <v>23</v>
       </c>
       <c r="C16" t="s">
-        <v>408</v>
+        <v>395</v>
       </c>
       <c r="D16" t="s">
         <v>131</v>
       </c>
       <c r="E16" t="s">
-        <v>478</v>
+        <v>465</v>
       </c>
       <c r="F16" t="s">
-        <v>478</v>
+        <v>465</v>
       </c>
       <c r="G16">
         <v>4599000</v>
@@ -2326,16 +2287,16 @@
         <v>24</v>
       </c>
       <c r="C17" t="s">
-        <v>409</v>
+        <v>396</v>
       </c>
       <c r="D17" t="s">
         <v>132</v>
       </c>
       <c r="E17" t="s">
-        <v>478</v>
+        <v>465</v>
       </c>
       <c r="F17" t="s">
-        <v>478</v>
+        <v>465</v>
       </c>
       <c r="G17">
         <v>6001500</v>
@@ -2355,16 +2316,16 @@
         <v>25</v>
       </c>
       <c r="C18" t="s">
-        <v>410</v>
+        <v>397</v>
       </c>
       <c r="D18" t="s">
         <v>133</v>
       </c>
       <c r="E18" t="s">
-        <v>478</v>
+        <v>465</v>
       </c>
       <c r="F18" t="s">
-        <v>478</v>
+        <v>465</v>
       </c>
       <c r="G18">
         <v>7001250</v>
@@ -2384,16 +2345,16 @@
         <v>26</v>
       </c>
       <c r="C19" t="s">
-        <v>411</v>
+        <v>398</v>
       </c>
       <c r="D19" t="s">
         <v>134</v>
       </c>
       <c r="E19" t="s">
-        <v>478</v>
+        <v>465</v>
       </c>
       <c r="F19" t="s">
-        <v>478</v>
+        <v>465</v>
       </c>
       <c r="G19">
         <v>8307000</v>
@@ -2413,16 +2374,16 @@
         <v>27</v>
       </c>
       <c r="C20" t="s">
-        <v>412</v>
+        <v>399</v>
       </c>
       <c r="D20" t="s">
         <v>135</v>
       </c>
       <c r="E20" t="s">
-        <v>478</v>
+        <v>465</v>
       </c>
       <c r="F20" t="s">
-        <v>478</v>
+        <v>465</v>
       </c>
       <c r="G20">
         <v>7663000</v>
@@ -2442,16 +2403,16 @@
         <v>28</v>
       </c>
       <c r="C21" t="s">
-        <v>413</v>
+        <v>400</v>
       </c>
       <c r="D21" t="s">
         <v>145</v>
       </c>
       <c r="E21" t="s">
-        <v>478</v>
+        <v>465</v>
       </c>
       <c r="F21" t="s">
-        <v>478</v>
+        <v>465</v>
       </c>
       <c r="G21">
         <v>15330000</v>
@@ -2471,16 +2432,16 @@
         <v>29</v>
       </c>
       <c r="C22" t="s">
-        <v>414</v>
+        <v>401</v>
       </c>
       <c r="D22" t="s">
         <v>136</v>
       </c>
       <c r="E22" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="F22" t="s">
-        <v>310</v>
+        <v>465</v>
       </c>
       <c r="G22">
         <v>5687000</v>
@@ -2500,16 +2461,16 @@
         <v>30</v>
       </c>
       <c r="C23" t="s">
-        <v>415</v>
+        <v>402</v>
       </c>
       <c r="D23" t="s">
         <v>137</v>
       </c>
       <c r="E23" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="F23" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="G23">
         <v>13600000</v>
@@ -2529,16 +2490,16 @@
         <v>31</v>
       </c>
       <c r="C24" t="s">
-        <v>416</v>
+        <v>403</v>
       </c>
       <c r="D24" t="s">
         <v>138</v>
       </c>
       <c r="E24" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="F24" t="s">
-        <v>312</v>
+        <v>465</v>
       </c>
       <c r="G24">
         <v>15943000</v>
@@ -2558,16 +2519,16 @@
         <v>32</v>
       </c>
       <c r="C25" t="s">
-        <v>417</v>
+        <v>404</v>
       </c>
       <c r="D25" t="s">
         <v>139</v>
       </c>
       <c r="E25" t="s">
-        <v>300</v>
+        <v>465</v>
       </c>
       <c r="F25" t="s">
-        <v>313</v>
+        <v>465</v>
       </c>
       <c r="G25">
         <v>15540000</v>
@@ -2587,16 +2548,16 @@
         <v>33</v>
       </c>
       <c r="C26" t="s">
-        <v>418</v>
+        <v>405</v>
       </c>
       <c r="D26" t="s">
         <v>140</v>
       </c>
       <c r="E26" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="F26" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="G26">
         <v>16586000</v>
@@ -2616,16 +2577,16 @@
         <v>34</v>
       </c>
       <c r="C27" t="s">
-        <v>419</v>
+        <v>406</v>
       </c>
       <c r="D27" t="s">
         <v>141</v>
       </c>
       <c r="E27" t="s">
-        <v>298</v>
+        <v>465</v>
       </c>
       <c r="F27" t="s">
-        <v>315</v>
+        <v>465</v>
       </c>
       <c r="G27">
         <v>9558000</v>
@@ -2645,16 +2606,16 @@
         <v>35</v>
       </c>
       <c r="C28" t="s">
-        <v>420</v>
+        <v>407</v>
       </c>
       <c r="D28" t="s">
         <v>142</v>
       </c>
       <c r="E28" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="F28" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="G28">
         <v>11792000</v>
@@ -2674,16 +2635,16 @@
         <v>36</v>
       </c>
       <c r="C29" t="s">
-        <v>421</v>
+        <v>408</v>
       </c>
       <c r="D29" t="s">
         <v>143</v>
       </c>
       <c r="E29" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="F29" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
       <c r="G29">
         <v>14030000</v>
@@ -2703,16 +2664,16 @@
         <v>37</v>
       </c>
       <c r="C30" t="s">
-        <v>422</v>
+        <v>409</v>
       </c>
       <c r="D30" t="s">
         <v>144</v>
       </c>
       <c r="E30" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="F30" t="s">
-        <v>318</v>
+        <v>309</v>
       </c>
       <c r="G30">
         <v>15348000</v>
@@ -2732,16 +2693,16 @@
         <v>38</v>
       </c>
       <c r="C31" t="s">
-        <v>423</v>
+        <v>410</v>
       </c>
       <c r="D31" t="s">
         <v>153</v>
       </c>
       <c r="E31" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="F31" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
       <c r="G31">
         <v>6185000</v>
@@ -2761,16 +2722,16 @@
         <v>39</v>
       </c>
       <c r="C32" t="s">
-        <v>453</v>
+        <v>440</v>
       </c>
       <c r="D32" t="s">
         <v>154</v>
       </c>
       <c r="E32" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="F32" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
       <c r="G32">
         <v>257000</v>
@@ -2790,16 +2751,16 @@
         <v>40</v>
       </c>
       <c r="C33" t="s">
-        <v>454</v>
+        <v>441</v>
       </c>
       <c r="D33" t="s">
         <v>155</v>
       </c>
       <c r="E33" t="s">
-        <v>292</v>
+        <v>465</v>
       </c>
       <c r="F33" t="s">
-        <v>321</v>
+        <v>465</v>
       </c>
       <c r="G33">
         <v>609000</v>
@@ -2819,16 +2780,16 @@
         <v>41</v>
       </c>
       <c r="C34" t="s">
-        <v>455</v>
+        <v>442</v>
       </c>
       <c r="D34" t="s">
         <v>156</v>
       </c>
       <c r="E34" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="F34" t="s">
-        <v>322</v>
+        <v>465</v>
       </c>
       <c r="G34">
         <v>537000</v>
@@ -2848,16 +2809,16 @@
         <v>42</v>
       </c>
       <c r="C35" t="s">
-        <v>456</v>
+        <v>443</v>
       </c>
       <c r="D35" t="s">
         <v>157</v>
       </c>
       <c r="E35" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="F35" t="s">
-        <v>323</v>
+        <v>312</v>
       </c>
       <c r="G35">
         <v>525000</v>
@@ -2877,16 +2838,16 @@
         <v>43</v>
       </c>
       <c r="C36" t="s">
-        <v>457</v>
+        <v>444</v>
       </c>
       <c r="D36" t="s">
         <v>158</v>
       </c>
       <c r="E36" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F36" t="s">
-        <v>324</v>
+        <v>313</v>
       </c>
       <c r="G36">
         <v>635000</v>
@@ -2906,16 +2867,16 @@
         <v>44</v>
       </c>
       <c r="C37" t="s">
-        <v>424</v>
+        <v>411</v>
       </c>
       <c r="D37" t="s">
         <v>159</v>
       </c>
       <c r="E37" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F37" t="s">
-        <v>325</v>
+        <v>314</v>
       </c>
       <c r="G37">
         <v>2621000</v>
@@ -2935,16 +2896,16 @@
         <v>45</v>
       </c>
       <c r="C38" t="s">
-        <v>425</v>
+        <v>412</v>
       </c>
       <c r="D38" t="s">
         <v>160</v>
       </c>
       <c r="E38" t="s">
-        <v>287</v>
+        <v>465</v>
       </c>
       <c r="F38" t="s">
-        <v>326</v>
+        <v>465</v>
       </c>
       <c r="G38">
         <v>5556000</v>
@@ -2964,16 +2925,16 @@
         <v>46</v>
       </c>
       <c r="C39" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="D39" t="s">
         <v>161</v>
       </c>
       <c r="E39" t="s">
-        <v>286</v>
+        <v>465</v>
       </c>
       <c r="F39" t="s">
-        <v>327</v>
+        <v>465</v>
       </c>
       <c r="G39">
         <v>6701000</v>
@@ -2993,7 +2954,7 @@
         <v>47</v>
       </c>
       <c r="C40" t="s">
-        <v>427</v>
+        <v>414</v>
       </c>
       <c r="D40" t="s">
         <v>162</v>
@@ -3002,7 +2963,7 @@
         <v>285</v>
       </c>
       <c r="F40" t="s">
-        <v>328</v>
+        <v>315</v>
       </c>
       <c r="G40">
         <v>9058000</v>
@@ -3022,7 +2983,7 @@
         <v>48</v>
       </c>
       <c r="C41" t="s">
-        <v>428</v>
+        <v>415</v>
       </c>
       <c r="D41" t="s">
         <v>146</v>
@@ -3031,7 +2992,7 @@
         <v>284</v>
       </c>
       <c r="F41" t="s">
-        <v>329</v>
+        <v>316</v>
       </c>
       <c r="G41">
         <v>3964000</v>
@@ -3051,7 +3012,7 @@
         <v>49</v>
       </c>
       <c r="C42" t="s">
-        <v>458</v>
+        <v>445</v>
       </c>
       <c r="D42" t="s">
         <v>147</v>
@@ -3060,7 +3021,7 @@
         <v>147</v>
       </c>
       <c r="F42" t="s">
-        <v>330</v>
+        <v>317</v>
       </c>
       <c r="G42">
         <v>485000</v>
@@ -3080,7 +3041,7 @@
         <v>50</v>
       </c>
       <c r="C43" t="s">
-        <v>459</v>
+        <v>446</v>
       </c>
       <c r="D43" t="s">
         <v>148</v>
@@ -3089,7 +3050,7 @@
         <v>283</v>
       </c>
       <c r="F43" t="s">
-        <v>331</v>
+        <v>318</v>
       </c>
       <c r="G43">
         <v>427000</v>
@@ -3109,7 +3070,7 @@
         <v>51</v>
       </c>
       <c r="C44" t="s">
-        <v>460</v>
+        <v>447</v>
       </c>
       <c r="D44" t="s">
         <v>149</v>
@@ -3118,7 +3079,7 @@
         <v>282</v>
       </c>
       <c r="F44" t="s">
-        <v>332</v>
+        <v>319</v>
       </c>
       <c r="G44">
         <v>551000</v>
@@ -3138,7 +3099,7 @@
         <v>52</v>
       </c>
       <c r="C45" t="s">
-        <v>461</v>
+        <v>448</v>
       </c>
       <c r="D45" t="s">
         <v>150</v>
@@ -3147,7 +3108,7 @@
         <v>281</v>
       </c>
       <c r="F45" t="s">
-        <v>333</v>
+        <v>320</v>
       </c>
       <c r="G45">
         <v>639000</v>
@@ -3167,7 +3128,7 @@
         <v>53</v>
       </c>
       <c r="C46" t="s">
-        <v>462</v>
+        <v>449</v>
       </c>
       <c r="D46" t="s">
         <v>151</v>
@@ -3176,7 +3137,7 @@
         <v>280</v>
       </c>
       <c r="F46" t="s">
-        <v>334</v>
+        <v>321</v>
       </c>
       <c r="G46">
         <v>661000</v>
@@ -3196,7 +3157,7 @@
         <v>54</v>
       </c>
       <c r="C47" t="s">
-        <v>463</v>
+        <v>450</v>
       </c>
       <c r="D47" t="s">
         <v>152</v>
@@ -3205,7 +3166,7 @@
         <v>279</v>
       </c>
       <c r="F47" t="s">
-        <v>335</v>
+        <v>322</v>
       </c>
       <c r="G47">
         <v>673000</v>
@@ -3225,7 +3186,7 @@
         <v>55</v>
       </c>
       <c r="C48" t="s">
-        <v>464</v>
+        <v>451</v>
       </c>
       <c r="D48" t="s">
         <v>163</v>
@@ -3234,7 +3195,7 @@
         <v>278</v>
       </c>
       <c r="F48" t="s">
-        <v>336</v>
+        <v>323</v>
       </c>
       <c r="G48">
         <v>445000</v>
@@ -3254,7 +3215,7 @@
         <v>56</v>
       </c>
       <c r="C49" t="s">
-        <v>465</v>
+        <v>452</v>
       </c>
       <c r="D49" t="s">
         <v>164</v>
@@ -3263,7 +3224,7 @@
         <v>277</v>
       </c>
       <c r="F49" t="s">
-        <v>337</v>
+        <v>324</v>
       </c>
       <c r="G49">
         <v>498000</v>
@@ -3283,7 +3244,7 @@
         <v>57</v>
       </c>
       <c r="C50" t="s">
-        <v>466</v>
+        <v>453</v>
       </c>
       <c r="D50" t="s">
         <v>165</v>
@@ -3292,7 +3253,7 @@
         <v>276</v>
       </c>
       <c r="F50" t="s">
-        <v>338</v>
+        <v>325</v>
       </c>
       <c r="G50">
         <v>546000</v>
@@ -3312,7 +3273,7 @@
         <v>58</v>
       </c>
       <c r="C51" t="s">
-        <v>467</v>
+        <v>454</v>
       </c>
       <c r="D51" t="s">
         <v>166</v>
@@ -3321,7 +3282,7 @@
         <v>275</v>
       </c>
       <c r="F51" t="s">
-        <v>339</v>
+        <v>326</v>
       </c>
       <c r="G51">
         <v>945000</v>
@@ -3341,7 +3302,7 @@
         <v>59</v>
       </c>
       <c r="C52" t="s">
-        <v>475</v>
+        <v>462</v>
       </c>
       <c r="D52" t="s">
         <v>213</v>
@@ -3350,7 +3311,7 @@
         <v>274</v>
       </c>
       <c r="F52" t="s">
-        <v>340</v>
+        <v>327</v>
       </c>
       <c r="G52">
         <v>1295000</v>
@@ -3370,7 +3331,7 @@
         <v>60</v>
       </c>
       <c r="C53" t="s">
-        <v>468</v>
+        <v>455</v>
       </c>
       <c r="D53" t="s">
         <v>167</v>
@@ -3379,7 +3340,7 @@
         <v>273</v>
       </c>
       <c r="F53" t="s">
-        <v>341</v>
+        <v>328</v>
       </c>
       <c r="G53">
         <v>857000</v>
@@ -3399,7 +3360,7 @@
         <v>61</v>
       </c>
       <c r="C54" t="s">
-        <v>469</v>
+        <v>456</v>
       </c>
       <c r="D54" t="s">
         <v>168</v>
@@ -3408,7 +3369,7 @@
         <v>272</v>
       </c>
       <c r="F54" t="s">
-        <v>342</v>
+        <v>329</v>
       </c>
       <c r="G54">
         <v>1045000</v>
@@ -3428,7 +3389,7 @@
         <v>62</v>
       </c>
       <c r="C55" t="s">
-        <v>470</v>
+        <v>457</v>
       </c>
       <c r="D55" t="s">
         <v>169</v>
@@ -3437,7 +3398,7 @@
         <v>271</v>
       </c>
       <c r="F55" t="s">
-        <v>343</v>
+        <v>330</v>
       </c>
       <c r="G55">
         <v>895000</v>
@@ -3457,7 +3418,7 @@
         <v>63</v>
       </c>
       <c r="C56" t="s">
-        <v>476</v>
+        <v>463</v>
       </c>
       <c r="D56" t="s">
         <v>170</v>
@@ -3466,7 +3427,7 @@
         <v>270</v>
       </c>
       <c r="F56" t="s">
-        <v>344</v>
+        <v>331</v>
       </c>
       <c r="G56">
         <v>1585000</v>
@@ -3486,7 +3447,7 @@
         <v>64</v>
       </c>
       <c r="C57" t="s">
-        <v>471</v>
+        <v>458</v>
       </c>
       <c r="D57" t="s">
         <v>171</v>
@@ -3495,7 +3456,7 @@
         <v>269</v>
       </c>
       <c r="F57" t="s">
-        <v>345</v>
+        <v>332</v>
       </c>
       <c r="G57">
         <v>1335000</v>
@@ -3515,7 +3476,7 @@
         <v>65</v>
       </c>
       <c r="C58" t="s">
-        <v>477</v>
+        <v>464</v>
       </c>
       <c r="D58" t="s">
         <v>172</v>
@@ -3524,7 +3485,7 @@
         <v>268</v>
       </c>
       <c r="F58" t="s">
-        <v>346</v>
+        <v>333</v>
       </c>
       <c r="G58">
         <v>1355000</v>
@@ -3544,7 +3505,7 @@
         <v>66</v>
       </c>
       <c r="C59" t="s">
-        <v>472</v>
+        <v>459</v>
       </c>
       <c r="D59" t="s">
         <v>173</v>
@@ -3553,7 +3514,7 @@
         <v>267</v>
       </c>
       <c r="F59" t="s">
-        <v>347</v>
+        <v>334</v>
       </c>
       <c r="G59">
         <v>745000</v>
@@ -3573,7 +3534,7 @@
         <v>67</v>
       </c>
       <c r="C60" t="s">
-        <v>473</v>
+        <v>460</v>
       </c>
       <c r="D60" t="s">
         <v>174</v>
@@ -3582,7 +3543,7 @@
         <v>266</v>
       </c>
       <c r="F60" t="s">
-        <v>348</v>
+        <v>335</v>
       </c>
       <c r="G60">
         <v>471000</v>
@@ -3602,7 +3563,7 @@
         <v>68</v>
       </c>
       <c r="C61" t="s">
-        <v>474</v>
+        <v>461</v>
       </c>
       <c r="D61" t="s">
         <v>175</v>
@@ -3611,7 +3572,7 @@
         <v>265</v>
       </c>
       <c r="F61" t="s">
-        <v>349</v>
+        <v>336</v>
       </c>
       <c r="G61">
         <v>1085000</v>
@@ -3628,7 +3589,7 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>391</v>
+        <v>378</v>
       </c>
       <c r="C62" t="s">
         <v>99</v>
@@ -3640,7 +3601,7 @@
         <v>264</v>
       </c>
       <c r="F62" t="s">
-        <v>350</v>
+        <v>337</v>
       </c>
       <c r="G62">
         <v>2468000</v>
@@ -3669,7 +3630,7 @@
         <v>263</v>
       </c>
       <c r="F63" t="s">
-        <v>351</v>
+        <v>338</v>
       </c>
       <c r="H63">
         <v>4</v>
@@ -3683,7 +3644,7 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>392</v>
+        <v>379</v>
       </c>
       <c r="C64" t="s">
         <v>101</v>
@@ -3695,7 +3656,7 @@
         <v>262</v>
       </c>
       <c r="F64" t="s">
-        <v>352</v>
+        <v>339</v>
       </c>
       <c r="G64">
         <v>8785000</v>
@@ -3712,7 +3673,7 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>393</v>
+        <v>380</v>
       </c>
       <c r="C65" t="s">
         <v>102</v>
@@ -3724,7 +3685,7 @@
         <v>261</v>
       </c>
       <c r="F65" t="s">
-        <v>353</v>
+        <v>340</v>
       </c>
       <c r="G65">
         <v>8930000</v>
@@ -3741,7 +3702,7 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>394</v>
+        <v>381</v>
       </c>
       <c r="C66" t="s">
         <v>103</v>
@@ -3753,7 +3714,7 @@
         <v>260</v>
       </c>
       <c r="F66" t="s">
-        <v>354</v>
+        <v>341</v>
       </c>
       <c r="G66">
         <v>7970000</v>
@@ -3782,7 +3743,7 @@
         <v>259</v>
       </c>
       <c r="F67" t="s">
-        <v>355</v>
+        <v>342</v>
       </c>
       <c r="G67">
         <v>2670000</v>
@@ -3799,7 +3760,7 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>395</v>
+        <v>382</v>
       </c>
       <c r="C68" t="s">
         <v>105</v>
@@ -3811,7 +3772,7 @@
         <v>258</v>
       </c>
       <c r="F68" t="s">
-        <v>356</v>
+        <v>343</v>
       </c>
       <c r="G68">
         <v>5420000</v>
@@ -3828,7 +3789,7 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>396</v>
+        <v>383</v>
       </c>
       <c r="C69" t="s">
         <v>106</v>
@@ -3840,7 +3801,7 @@
         <v>257</v>
       </c>
       <c r="F69" t="s">
-        <v>357</v>
+        <v>344</v>
       </c>
       <c r="G69">
         <v>4550000</v>
@@ -3857,7 +3818,7 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>397</v>
+        <v>384</v>
       </c>
       <c r="C70" t="s">
         <v>107</v>
@@ -3869,7 +3830,7 @@
         <v>256</v>
       </c>
       <c r="F70" t="s">
-        <v>358</v>
+        <v>345</v>
       </c>
       <c r="G70">
         <v>4840000</v>
@@ -3886,7 +3847,7 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>398</v>
+        <v>385</v>
       </c>
       <c r="C71" t="s">
         <v>108</v>
@@ -3898,7 +3859,7 @@
         <v>255</v>
       </c>
       <c r="F71" t="s">
-        <v>359</v>
+        <v>346</v>
       </c>
       <c r="G71">
         <v>4530000</v>
@@ -3927,7 +3888,7 @@
         <v>254</v>
       </c>
       <c r="F72" t="s">
-        <v>360</v>
+        <v>347</v>
       </c>
       <c r="G72">
         <v>2400000</v>
@@ -3956,7 +3917,7 @@
         <v>253</v>
       </c>
       <c r="F73" t="s">
-        <v>361</v>
+        <v>348</v>
       </c>
       <c r="G73">
         <v>2360000</v>
@@ -3985,7 +3946,7 @@
         <v>252</v>
       </c>
       <c r="F74" t="s">
-        <v>362</v>
+        <v>349</v>
       </c>
       <c r="G74">
         <v>2468000</v>
@@ -4014,7 +3975,7 @@
         <v>251</v>
       </c>
       <c r="F75" t="s">
-        <v>363</v>
+        <v>350</v>
       </c>
       <c r="G75">
         <v>2468000</v>
@@ -4043,7 +4004,7 @@
         <v>250</v>
       </c>
       <c r="F76" t="s">
-        <v>364</v>
+        <v>351</v>
       </c>
       <c r="G76">
         <v>2468000</v>
@@ -4072,7 +4033,7 @@
         <v>249</v>
       </c>
       <c r="F77" t="s">
-        <v>365</v>
+        <v>352</v>
       </c>
       <c r="G77">
         <v>2562000</v>
@@ -4101,7 +4062,7 @@
         <v>248</v>
       </c>
       <c r="F78" t="s">
-        <v>366</v>
+        <v>353</v>
       </c>
       <c r="G78">
         <v>2562000</v>
@@ -4130,7 +4091,7 @@
         <v>247</v>
       </c>
       <c r="F79" t="s">
-        <v>367</v>
+        <v>354</v>
       </c>
       <c r="G79">
         <v>2670000</v>
@@ -4159,7 +4120,7 @@
         <v>246</v>
       </c>
       <c r="F80" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="G80">
         <v>2773000</v>
@@ -4188,7 +4149,7 @@
         <v>245</v>
       </c>
       <c r="F81" t="s">
-        <v>369</v>
+        <v>356</v>
       </c>
       <c r="G81">
         <v>2773000</v>
@@ -4217,7 +4178,7 @@
         <v>244</v>
       </c>
       <c r="F82" t="s">
-        <v>370</v>
+        <v>357</v>
       </c>
       <c r="G82">
         <v>2810000</v>
@@ -4237,7 +4198,7 @@
         <v>80</v>
       </c>
       <c r="C83" t="s">
-        <v>429</v>
+        <v>416</v>
       </c>
       <c r="D83" t="s">
         <v>197</v>
@@ -4246,7 +4207,7 @@
         <v>243</v>
       </c>
       <c r="F83" t="s">
-        <v>371</v>
+        <v>358</v>
       </c>
       <c r="G83">
         <v>1080000</v>
@@ -4266,7 +4227,7 @@
         <v>81</v>
       </c>
       <c r="C84" t="s">
-        <v>430</v>
+        <v>417</v>
       </c>
       <c r="D84" t="s">
         <v>198</v>
@@ -4275,7 +4236,7 @@
         <v>242</v>
       </c>
       <c r="F84" t="s">
-        <v>372</v>
+        <v>359</v>
       </c>
       <c r="G84">
         <v>1322000</v>
@@ -4295,7 +4256,7 @@
         <v>82</v>
       </c>
       <c r="C85" t="s">
-        <v>431</v>
+        <v>418</v>
       </c>
       <c r="D85" t="s">
         <v>199</v>
@@ -4304,7 +4265,7 @@
         <v>241</v>
       </c>
       <c r="F85" t="s">
-        <v>373</v>
+        <v>360</v>
       </c>
       <c r="G85">
         <v>1717000</v>
@@ -4324,7 +4285,7 @@
         <v>83</v>
       </c>
       <c r="C86" t="s">
-        <v>432</v>
+        <v>419</v>
       </c>
       <c r="D86" t="s">
         <v>200</v>
@@ -4333,7 +4294,7 @@
         <v>240</v>
       </c>
       <c r="F86" t="s">
-        <v>374</v>
+        <v>361</v>
       </c>
       <c r="G86">
         <v>2341000</v>
@@ -4353,7 +4314,7 @@
         <v>84</v>
       </c>
       <c r="C87" t="s">
-        <v>433</v>
+        <v>420</v>
       </c>
       <c r="D87" t="s">
         <v>201</v>
@@ -4362,7 +4323,7 @@
         <v>239</v>
       </c>
       <c r="F87" t="s">
-        <v>375</v>
+        <v>362</v>
       </c>
       <c r="G87">
         <v>2175000</v>
@@ -4382,7 +4343,7 @@
         <v>85</v>
       </c>
       <c r="C88" t="s">
-        <v>434</v>
+        <v>421</v>
       </c>
       <c r="D88" t="s">
         <v>202</v>
@@ -4391,7 +4352,7 @@
         <v>238</v>
       </c>
       <c r="F88" t="s">
-        <v>376</v>
+        <v>363</v>
       </c>
       <c r="G88">
         <v>1862000</v>
@@ -4411,7 +4372,7 @@
         <v>86</v>
       </c>
       <c r="C89" t="s">
-        <v>435</v>
+        <v>422</v>
       </c>
       <c r="D89" t="s">
         <v>203</v>
@@ -4420,7 +4381,7 @@
         <v>237</v>
       </c>
       <c r="F89" t="s">
-        <v>377</v>
+        <v>364</v>
       </c>
       <c r="G89">
         <v>6713000</v>
@@ -4440,7 +4401,7 @@
         <v>87</v>
       </c>
       <c r="C90" t="s">
-        <v>436</v>
+        <v>423</v>
       </c>
       <c r="D90" t="s">
         <v>204</v>
@@ -4449,7 +4410,7 @@
         <v>236</v>
       </c>
       <c r="F90" t="s">
-        <v>378</v>
+        <v>365</v>
       </c>
       <c r="G90">
         <v>6627000</v>
@@ -4469,7 +4430,7 @@
         <v>88</v>
       </c>
       <c r="C91" t="s">
-        <v>437</v>
+        <v>424</v>
       </c>
       <c r="D91" t="s">
         <v>205</v>
@@ -4478,7 +4439,7 @@
         <v>235</v>
       </c>
       <c r="F91" t="s">
-        <v>379</v>
+        <v>366</v>
       </c>
       <c r="G91">
         <v>20615000</v>
@@ -4498,7 +4459,7 @@
         <v>89</v>
       </c>
       <c r="C92" t="s">
-        <v>438</v>
+        <v>425</v>
       </c>
       <c r="D92" t="s">
         <v>206</v>
@@ -4507,7 +4468,7 @@
         <v>234</v>
       </c>
       <c r="F92" t="s">
-        <v>380</v>
+        <v>367</v>
       </c>
       <c r="G92">
         <v>9275000</v>
@@ -4527,7 +4488,7 @@
         <v>90</v>
       </c>
       <c r="C93" t="s">
-        <v>439</v>
+        <v>426</v>
       </c>
       <c r="D93" t="s">
         <v>207</v>
@@ -4536,7 +4497,7 @@
         <v>233</v>
       </c>
       <c r="F93" t="s">
-        <v>381</v>
+        <v>368</v>
       </c>
       <c r="G93">
         <v>10326000</v>
@@ -4556,7 +4517,7 @@
         <v>91</v>
       </c>
       <c r="C94" t="s">
-        <v>440</v>
+        <v>427</v>
       </c>
       <c r="D94" t="s">
         <v>208</v>
@@ -4565,7 +4526,7 @@
         <v>232</v>
       </c>
       <c r="F94" t="s">
-        <v>382</v>
+        <v>369</v>
       </c>
       <c r="G94">
         <v>10691000</v>
@@ -4585,7 +4546,7 @@
         <v>92</v>
       </c>
       <c r="C95" t="s">
-        <v>441</v>
+        <v>428</v>
       </c>
       <c r="D95" t="s">
         <v>209</v>
@@ -4594,7 +4555,7 @@
         <v>231</v>
       </c>
       <c r="F95" t="s">
-        <v>383</v>
+        <v>370</v>
       </c>
       <c r="G95">
         <v>68528000</v>
@@ -4614,7 +4575,7 @@
         <v>93</v>
       </c>
       <c r="C96" t="s">
-        <v>442</v>
+        <v>429</v>
       </c>
       <c r="D96" t="s">
         <v>210</v>
@@ -4623,7 +4584,7 @@
         <v>230</v>
       </c>
       <c r="F96" t="s">
-        <v>384</v>
+        <v>371</v>
       </c>
       <c r="G96">
         <v>10342000</v>
@@ -4643,7 +4604,7 @@
         <v>94</v>
       </c>
       <c r="C97" t="s">
-        <v>443</v>
+        <v>430</v>
       </c>
       <c r="D97" t="s">
         <v>211</v>
@@ -4652,7 +4613,7 @@
         <v>229</v>
       </c>
       <c r="F97" t="s">
-        <v>385</v>
+        <v>372</v>
       </c>
       <c r="G97">
         <v>2441000</v>
@@ -4672,7 +4633,7 @@
         <v>95</v>
       </c>
       <c r="C98" t="s">
-        <v>444</v>
+        <v>431</v>
       </c>
       <c r="D98" t="s">
         <v>214</v>
@@ -4681,7 +4642,7 @@
         <v>228</v>
       </c>
       <c r="F98" t="s">
-        <v>386</v>
+        <v>373</v>
       </c>
       <c r="G98">
         <v>1826000</v>
@@ -4701,7 +4662,7 @@
         <v>96</v>
       </c>
       <c r="C99" t="s">
-        <v>445</v>
+        <v>432</v>
       </c>
       <c r="D99" t="s">
         <v>215</v>
@@ -4710,7 +4671,7 @@
         <v>227</v>
       </c>
       <c r="F99" t="s">
-        <v>387</v>
+        <v>374</v>
       </c>
       <c r="G99">
         <v>2450000</v>
@@ -4730,7 +4691,7 @@
         <v>97</v>
       </c>
       <c r="C100" t="s">
-        <v>446</v>
+        <v>433</v>
       </c>
       <c r="D100" t="s">
         <v>216</v>
@@ -4739,7 +4700,7 @@
         <v>226</v>
       </c>
       <c r="F100" t="s">
-        <v>388</v>
+        <v>375</v>
       </c>
       <c r="G100">
         <v>10346000</v>
@@ -4759,7 +4720,7 @@
         <v>98</v>
       </c>
       <c r="C101" t="s">
-        <v>447</v>
+        <v>434</v>
       </c>
       <c r="D101" t="s">
         <v>212</v>
@@ -4768,7 +4729,7 @@
         <v>225</v>
       </c>
       <c r="F101" t="s">
-        <v>389</v>
+        <v>376</v>
       </c>
       <c r="G101">
         <v>5723000</v>

</xml_diff>